<commit_message>
Configuration management procedure aligned
with GitHub
new template CM plan
Project plan procedure
QMS change requirements template
</commit_message>
<xml_diff>
--- a/Process Management/TMPL_QMSREQ.xlsx
+++ b/Process Management/TMPL_QMSREQ.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Revision History" sheetId="1" r:id="rId1"/>
@@ -48,13 +48,13 @@
     <t>Instructions for Use</t>
   </si>
   <si>
-    <t>SVN Repository Rev.</t>
-  </si>
-  <si>
-    <t>Template Version -2</t>
-  </si>
-  <si>
     <t>Points to cover in Post Release training</t>
+  </si>
+  <si>
+    <t>Template Version -3</t>
+  </si>
+  <si>
+    <t>Repository Rev.</t>
   </si>
 </sst>
 </file>
@@ -162,7 +162,7 @@
     <tableColumn id="7" name="Artefacts to be modified"/>
     <tableColumn id="8" name="Size"/>
     <tableColumn id="5" name="Remarks"/>
-    <tableColumn id="6" name="SVN Repository Rev."/>
+    <tableColumn id="6" name="Repository Rev."/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -457,7 +457,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -501,8 +503,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:H16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -544,12 +546,12 @@
         <v>5</v>
       </c>
       <c r="H5" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>